<commit_message>
finished examining the error during reaching. gonna do the reflex experiments
</commit_message>
<xml_diff>
--- a/data/voltage_force_slope/calculate_new_parameters.xlsx
+++ b/data/voltage_force_slope/calculate_new_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mizuki\University\Reserch\reflex\control_board_Mizuki\data\voltage_force_slope\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E94B84FA-A954-4A25-8186-31BDD38872F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9644843B-A0FE-4BEB-B453-B981C5D48FD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28905" yWindow="-2580" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="16">
   <si>
     <t>a_3_agonist</t>
     <phoneticPr fontId="1"/>
@@ -71,6 +71,33 @@
   </si>
   <si>
     <t>ant_force_voltage_slope</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ave</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2024/08/12（直接フォースゲージつけた）</t>
+    <rPh sb="11" eb="13">
+      <t>チョクセツ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ago_force</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ago_voltage</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>anta_force</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>anta_voltage</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -399,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:M40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="E19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M37" sqref="M37:M40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -527,8 +554,394 @@
         <v>586.59965205000003</v>
       </c>
     </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="1">
+        <v>45515</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>98.836269999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>-83.661230000000003</v>
+      </c>
+      <c r="E16">
+        <v>98.916240000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="D17">
+        <v>-67.876499999999993</v>
+      </c>
+      <c r="E17">
+        <v>76.397530000000003</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="C18">
+        <v>4</v>
+      </c>
+      <c r="D18">
+        <v>-87.812299999999993</v>
+      </c>
+      <c r="E18">
+        <v>73.182720000000003</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="C19">
+        <v>5</v>
+      </c>
+      <c r="D19">
+        <v>-126.319</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="C20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20">
+        <f>AVERAGE(D15:D19)</f>
+        <v>-91.417257500000005</v>
+      </c>
+      <c r="E20">
+        <f>AVERAGE(E15:E18)</f>
+        <v>86.833190000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23">
+        <v>-0.20082</v>
+      </c>
+      <c r="D23">
+        <f>B23*$D$20</f>
+        <v>18.358413651150002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24">
+        <v>7.001792</v>
+      </c>
+      <c r="D24">
+        <f t="shared" ref="D24:D26" si="2">B24*$D$20</f>
+        <v>-640.08462222544006</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>2</v>
+      </c>
+      <c r="B25">
+        <v>0.25617299999999998</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="2"/>
+        <v>-23.418633105547499</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26">
+        <v>0.91102000000000005</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="2"/>
+        <v>-83.282949927650009</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27">
+        <v>0.245392</v>
+      </c>
+      <c r="E27">
+        <f>B27*$E$20</f>
+        <v>21.30817016048</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28">
+        <v>0.34852100000000003</v>
+      </c>
+      <c r="E28">
+        <f t="shared" ref="E28:E30" si="3">B28*$E$20</f>
+        <v>30.263190211990004</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29">
+        <v>-3.6479999999999999E-2</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="3"/>
+        <v>-3.1676747711999997</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30">
+        <v>6.3177130000000004</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="3"/>
+        <v>548.58717329447006</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13">
+      <c r="A33" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33">
+        <v>-0.20082</v>
+      </c>
+      <c r="D33" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33" t="s">
+        <v>13</v>
+      </c>
+      <c r="H33" t="s">
+        <v>14</v>
+      </c>
+      <c r="I33" t="s">
+        <v>15</v>
+      </c>
+      <c r="L33">
+        <f>B33*$F$39</f>
+        <v>0.36906225672194332</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13">
+      <c r="A34" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34">
+        <v>7.001792</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="H34">
+        <v>11.9</v>
+      </c>
+      <c r="I34">
+        <v>39</v>
+      </c>
+      <c r="J34">
+        <f>I34/H34</f>
+        <v>3.2773109243697478</v>
+      </c>
+      <c r="L34">
+        <f t="shared" ref="L34:L38" si="4">B34*$F$39</f>
+        <v>-12.867728097886909</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
+      <c r="A35" t="s">
+        <v>2</v>
+      </c>
+      <c r="B35">
+        <v>0.25617299999999998</v>
+      </c>
+      <c r="C35">
+        <v>2</v>
+      </c>
+      <c r="D35">
+        <v>22.9</v>
+      </c>
+      <c r="E35">
+        <v>-48</v>
+      </c>
+      <c r="F35">
+        <f>E35/D35</f>
+        <v>-2.0960698689956332</v>
+      </c>
+      <c r="L35">
+        <f>B35*$F$39</f>
+        <v>-0.47078869381152461</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13">
+      <c r="A36" t="s">
+        <v>3</v>
+      </c>
+      <c r="B36">
+        <v>0.91102000000000005</v>
+      </c>
+      <c r="C36">
+        <v>3</v>
+      </c>
+      <c r="D36">
+        <v>20.6</v>
+      </c>
+      <c r="E36">
+        <v>-27</v>
+      </c>
+      <c r="F36">
+        <f t="shared" ref="F36:F38" si="5">E36/D36</f>
+        <v>-1.3106796116504853</v>
+      </c>
+      <c r="H36">
+        <v>10.9</v>
+      </c>
+      <c r="I36">
+        <v>34</v>
+      </c>
+      <c r="J36">
+        <f t="shared" ref="J35:J38" si="6">I36/H36</f>
+        <v>3.1192660550458715</v>
+      </c>
+      <c r="L36">
+        <f t="shared" si="4"/>
+        <v>-1.6742510562634438</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
+      <c r="A37" t="s">
+        <v>4</v>
+      </c>
+      <c r="B37">
+        <v>0.245392</v>
+      </c>
+      <c r="C37">
+        <v>4</v>
+      </c>
+      <c r="D37">
+        <v>18.5</v>
+      </c>
+      <c r="E37">
+        <v>-24</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="5"/>
+        <v>-1.2972972972972974</v>
+      </c>
+      <c r="H37">
+        <v>12.4</v>
+      </c>
+      <c r="I37">
+        <v>45</v>
+      </c>
+      <c r="J37">
+        <f>I37/H37</f>
+        <v>3.629032258064516</v>
+      </c>
+      <c r="M37">
+        <f>B37*$J$39</f>
+        <v>0.87066774216759812</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
+      <c r="A38" t="s">
+        <v>5</v>
+      </c>
+      <c r="B38">
+        <v>0.34852100000000003</v>
+      </c>
+      <c r="C38">
+        <v>5</v>
+      </c>
+      <c r="D38">
+        <v>23.8</v>
+      </c>
+      <c r="E38">
+        <v>-63</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="5"/>
+        <v>-2.6470588235294117</v>
+      </c>
+      <c r="H38">
+        <v>12</v>
+      </c>
+      <c r="I38">
+        <v>50</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="6"/>
+        <v>4.166666666666667</v>
+      </c>
+      <c r="M38">
+        <f t="shared" ref="M38:M40" si="7">B38*$J$39</f>
+        <v>1.2365765475972872</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13">
+      <c r="A39" t="s">
+        <v>6</v>
+      </c>
+      <c r="B39">
+        <v>-3.6479999999999999E-2</v>
+      </c>
+      <c r="F39">
+        <f>AVERAGE(F35:F38)</f>
+        <v>-1.8377764003682069</v>
+      </c>
+      <c r="J39">
+        <f>AVERAGE(J34:J38)</f>
+        <v>3.548068976036701</v>
+      </c>
+      <c r="M39">
+        <f t="shared" si="7"/>
+        <v>-0.12943355624581884</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13">
+      <c r="A40" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40">
+        <v>6.3177130000000004</v>
+      </c>
+      <c r="M40">
+        <f t="shared" si="7"/>
+        <v>22.415681494803756</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
finished examining reaching error in a new system, gonnna do the reflex exeriments
</commit_message>
<xml_diff>
--- a/data/voltage_force_slope/calculate_new_parameters.xlsx
+++ b/data/voltage_force_slope/calculate_new_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mizuki\University\Reserch\reflex\control_board_Mizuki\data\voltage_force_slope\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9644843B-A0FE-4BEB-B453-B981C5D48FD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D65E46E8-0AD8-442C-964D-C7E9BF4A045B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28905" yWindow="-2580" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="17">
   <si>
     <t>a_3_agonist</t>
     <phoneticPr fontId="1"/>
@@ -98,6 +98,13 @@
   </si>
   <si>
     <t>anta_voltage</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2024/08/18（直接フォースゲージつけた）</t>
+    <rPh sb="11" eb="13">
+      <t>チョクセツ</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -426,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M40"/>
+  <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M37" sqref="M37:M40"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L43" sqref="L43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -773,7 +780,7 @@
         <v>3.2773109243697478</v>
       </c>
       <c r="L34">
-        <f t="shared" ref="L34:L38" si="4">B34*$F$39</f>
+        <f t="shared" ref="L34:L36" si="4">B34*$F$39</f>
         <v>-12.867728097886909</v>
       </c>
     </row>
@@ -829,7 +836,7 @@
         <v>34</v>
       </c>
       <c r="J36">
-        <f t="shared" ref="J35:J38" si="6">I36/H36</f>
+        <f t="shared" ref="J36:J38" si="6">I36/H36</f>
         <v>3.1192660550458715</v>
       </c>
       <c r="L36">
@@ -937,6 +944,242 @@
       <c r="M40">
         <f t="shared" si="7"/>
         <v>22.415681494803756</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13">
+      <c r="A42" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13">
+      <c r="A43" t="s">
+        <v>0</v>
+      </c>
+      <c r="B43">
+        <v>-0.20082</v>
+      </c>
+      <c r="D43" t="s">
+        <v>12</v>
+      </c>
+      <c r="E43" t="s">
+        <v>13</v>
+      </c>
+      <c r="H43" t="s">
+        <v>14</v>
+      </c>
+      <c r="I43" t="s">
+        <v>15</v>
+      </c>
+      <c r="L43">
+        <f>B43*$F$49</f>
+        <v>3.5454569514903564</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13">
+      <c r="A44" t="s">
+        <v>1</v>
+      </c>
+      <c r="B44">
+        <v>7.001792</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="D44">
+        <v>5.8</v>
+      </c>
+      <c r="E44">
+        <v>-92</v>
+      </c>
+      <c r="F44">
+        <f>E44/D44</f>
+        <v>-15.862068965517242</v>
+      </c>
+      <c r="H44">
+        <v>3.1</v>
+      </c>
+      <c r="I44">
+        <v>118</v>
+      </c>
+      <c r="J44">
+        <f>I44/H44</f>
+        <v>38.064516129032256</v>
+      </c>
+      <c r="L44">
+        <f>B44*$F$49</f>
+        <v>-123.61593526187414</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13">
+      <c r="A45" t="s">
+        <v>2</v>
+      </c>
+      <c r="B45">
+        <v>0.25617299999999998</v>
+      </c>
+      <c r="C45">
+        <v>2</v>
+      </c>
+      <c r="D45">
+        <v>6</v>
+      </c>
+      <c r="E45">
+        <v>-124</v>
+      </c>
+      <c r="F45">
+        <f t="shared" ref="F45:F48" si="8">E45/D45</f>
+        <v>-20.666666666666668</v>
+      </c>
+      <c r="H45">
+        <v>3.1</v>
+      </c>
+      <c r="I45">
+        <v>122</v>
+      </c>
+      <c r="J45">
+        <f t="shared" ref="J45:J48" si="9">I45/H45</f>
+        <v>39.354838709677416</v>
+      </c>
+      <c r="L45">
+        <f>B45*$F$49</f>
+        <v>-4.5227086128579774</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13">
+      <c r="A46" t="s">
+        <v>3</v>
+      </c>
+      <c r="B46">
+        <v>0.91102000000000005</v>
+      </c>
+      <c r="C46">
+        <v>3</v>
+      </c>
+      <c r="D46">
+        <v>5.9</v>
+      </c>
+      <c r="E46">
+        <v>-112</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="8"/>
+        <v>-18.983050847457626</v>
+      </c>
+      <c r="H46">
+        <v>3.6</v>
+      </c>
+      <c r="I46">
+        <v>152</v>
+      </c>
+      <c r="J46">
+        <f t="shared" si="9"/>
+        <v>42.222222222222221</v>
+      </c>
+      <c r="L46">
+        <f>B46*$F$49</f>
+        <v>-16.083966696278978</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13">
+      <c r="A47" t="s">
+        <v>4</v>
+      </c>
+      <c r="B47">
+        <v>0.245392</v>
+      </c>
+      <c r="C47">
+        <v>4</v>
+      </c>
+      <c r="D47">
+        <v>5.9</v>
+      </c>
+      <c r="E47">
+        <v>-93</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="8"/>
+        <v>-15.762711864406779</v>
+      </c>
+      <c r="H47">
+        <v>3.7</v>
+      </c>
+      <c r="I47">
+        <v>135</v>
+      </c>
+      <c r="J47">
+        <f t="shared" si="9"/>
+        <v>36.486486486486484</v>
+      </c>
+      <c r="M47">
+        <f>B47*$J$49</f>
+        <v>9.6643976592687757</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13">
+      <c r="A48" t="s">
+        <v>5</v>
+      </c>
+      <c r="B48">
+        <v>0.34852100000000003</v>
+      </c>
+      <c r="C48">
+        <v>5</v>
+      </c>
+      <c r="D48">
+        <v>6</v>
+      </c>
+      <c r="E48">
+        <v>-102</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="8"/>
+        <v>-17</v>
+      </c>
+      <c r="H48">
+        <v>3.8</v>
+      </c>
+      <c r="I48">
+        <v>155</v>
+      </c>
+      <c r="J48">
+        <f t="shared" si="9"/>
+        <v>40.789473684210527</v>
+      </c>
+      <c r="M48">
+        <f>B48*$J$49</f>
+        <v>13.725979398700908</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13">
+      <c r="A49" t="s">
+        <v>6</v>
+      </c>
+      <c r="B49">
+        <v>-3.6479999999999999E-2</v>
+      </c>
+      <c r="F49">
+        <f>AVERAGE(F44:F48)</f>
+        <v>-17.654899668809662</v>
+      </c>
+      <c r="J49">
+        <f>AVERAGE(J44:J48)</f>
+        <v>39.38350744632578</v>
+      </c>
+      <c r="M49">
+        <f>B49*$J$49</f>
+        <v>-1.4367103516419644</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13">
+      <c r="A50" t="s">
+        <v>7</v>
+      </c>
+      <c r="B50">
+        <v>6.3177130000000004</v>
+      </c>
+      <c r="M50">
+        <f>B50*$J$49</f>
+        <v>248.81369697924919</v>
       </c>
     </row>
   </sheetData>

</xml_diff>